<commit_message>
Added chart to domestic violence data
</commit_message>
<xml_diff>
--- a/excel/sql_query_output.xlsx
+++ b/excel/sql_query_output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime\Desktop\git-repo\chicago_crime_and_weather_2021\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596C365D-8AE0-439B-B68D-4772C2CC05E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB70177-A0FB-42AA-9483-1532E275945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="8" activeTab="12" xr2:uid="{CE6839DA-4336-434C-A3C6-5CF43E49803F}"/>
+    <workbookView xWindow="-28920" yWindow="-705" windowWidth="28110" windowHeight="16440" activeTab="3" xr2:uid="{CE6839DA-4336-434C-A3C6-5CF43E49803F}"/>
   </bookViews>
   <sheets>
     <sheet name="consecutive_homicide" sheetId="2" r:id="rId1"/>
@@ -42,6 +42,9 @@
     <definedName name="ExternalData_1" localSheetId="11" hidden="1">top_streets_homicide!$B$1:$B$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="1" r:id="rId14"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -103,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
   <si>
     <t>most_consecutive_days</t>
   </si>
@@ -367,6 +370,12 @@
   </si>
   <si>
     <t>North Park.</t>
+  </si>
+  <si>
+    <t>Sum of domestic_violence</t>
+  </si>
+  <si>
+    <t>Sum of non_domestic_violence</t>
   </si>
 </sst>
 </file>
@@ -453,6 +462,1680 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[sql_query_output.xlsx]domestic_violence!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:fld id="{AB21EB55-3B76-4072-A7FF-49CD87ECBA50}" type="VALUE">
+                  <a:rPr lang="en-US" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="95000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:pPr>
+                    <a:defRPr sz="1100"/>
+                  </a:pPr>
+                  <a:t>[VALUE]</a:t>
+                </a:fld>
+                <a:r>
+                  <a:rPr lang="en-US" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="95000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>%</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:dlblFieldTable/>
+              <c15:showDataLabelsRange val="0"/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:fld id="{3E1F0BED-2A40-4094-A140-9DA472C90CE3}" type="VALUE">
+                  <a:rPr lang="en-US" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="95000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:pPr>
+                    <a:defRPr sz="1100"/>
+                  </a:pPr>
+                  <a:t>[VALUE]</a:t>
+                </a:fld>
+                <a:r>
+                  <a:rPr lang="en-US" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="95000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>%</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:dlblFieldTable/>
+              <c15:showDataLabelsRange val="0"/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>domestic_violence!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum of domestic_violence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{3E1F0BED-2A40-4094-A140-9DA472C90CE3}" type="VALUE">
+                      <a:rPr lang="en-US" b="1">
+                        <a:solidFill>
+                          <a:schemeClr val="bg1">
+                            <a:lumMod val="95000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" b="1">
+                        <a:solidFill>
+                          <a:schemeClr val="bg1">
+                            <a:lumMod val="95000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-82E7-4BE7-A3BC-3EED7278D295}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>domestic_violence!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>domestic_violence!$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>21.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-82E7-4BE7-A3BC-3EED7278D295}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>domestic_violence!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum of non_domestic_violence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-82E7-4BE7-A3BC-3EED7278D295}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{AB21EB55-3B76-4072-A7FF-49CD87ECBA50}" type="VALUE">
+                      <a:rPr lang="en-US" b="1">
+                        <a:solidFill>
+                          <a:schemeClr val="bg1">
+                            <a:lumMod val="95000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" b="1">
+                        <a:solidFill>
+                          <a:schemeClr val="bg1">
+                            <a:lumMod val="95000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-82E7-4BE7-A3BC-3EED7278D295}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>domestic_violence!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>domestic_violence!$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>78.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-82E7-4BE7-A3BC-3EED7278D295}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="935316559"/>
+        <c:axId val="935307407"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="935316559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="935307407"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="935307407"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="935316559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="Group 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ECB65B6-92EB-5FA9-6863-9A12A70BB939}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3867150" y="828675"/>
+          <a:ext cx="3667125" cy="2076450"/>
+          <a:chOff x="4714875" y="981075"/>
+          <a:chExt cx="3667125" cy="2076450"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Rectangle: Rounded Corners 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{120C586F-D25E-FFD9-4C4C-1EC5A968EE24}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4714875" y="981075"/>
+            <a:ext cx="3095625" cy="1990725"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 4000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:gradFill flip="none" rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="75000"/>
+                  <a:shade val="30000"/>
+                  <a:satMod val="115000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="75000"/>
+                  <a:shade val="67500"/>
+                  <a:satMod val="115000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="75000"/>
+                  <a:shade val="100000"/>
+                  <a:satMod val="115000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="2700000" scaled="1"/>
+            <a:tileRect/>
+          </a:gradFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="3" name="Chart 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E75A497-73D7-DABB-A75B-620C67F74D1B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="5591175" y="1057275"/>
+          <a:ext cx="2790825" cy="2000250"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="TextBox 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E56AF6E6-331F-B247-39D2-245C2162711E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4857750" y="1171574"/>
+            <a:ext cx="2162175" cy="655949"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Over </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>20%</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> of all reported</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> crimes where some form of domestic violence.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jaime" refreshedDate="44933.870074537037" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{BD78492D-6275-42DE-A6FF-A763F864DB1E}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="domestic_violence"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="non_domestic_violence" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="78.2" maxValue="78.2"/>
+    </cacheField>
+    <cacheField name="domestic_violence" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="21.8" maxValue="21.8"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
+  <r>
+    <n v="78.2"/>
+    <n v="21.8"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7400F035-ADCB-442E-9D3B-CA40FF32DF26}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="D2:E3" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of domestic_violence" fld="1" baseField="0" baseItem="0"/>
+    <dataField name="Sum of non_domestic_violence" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{B339FC43-C7A9-431D-B02B-4C015CB1B26B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="3">
@@ -624,7 +2307,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E3BC32D3-E9CB-4FB9-9F98-7D59A879005B}" name="top_crime_weekday" displayName="top_crime_weekday" ref="A1:B8" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B8" xr:uid="{E3BC32D3-E9CB-4FB9-9F98-7D59A879005B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{AD5E170E-73C4-454E-82B1-7DA81A6EFCD6}" uniqueName="1" name="day_of_week" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{AD5E170E-73C4-454E-82B1-7DA81A6EFCD6}" uniqueName="1" name="day_of_week" queryTableFieldId="1" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{C9E87FF3-75EF-4377-85FE-178D46DAA5F2}" uniqueName="2" name="n_crimes" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -635,7 +2318,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0D92DAAA-F6FE-4B2E-A008-6757307FA6F8}" name="top_month_homicide" displayName="top_month_homicide" ref="A1:D13" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D13" xr:uid="{0D92DAAA-F6FE-4B2E-A008-6757307FA6F8}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{64A4C862-9E4C-410F-943B-F731E46517EB}" uniqueName="1" name="month" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{64A4C862-9E4C-410F-943B-F731E46517EB}" uniqueName="1" name="month" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{2BE5E1AF-87B9-46BA-8E84-007DB57234B9}" uniqueName="2" name="n_homicides" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{4A4D9BAB-E3DB-4685-939B-77B2472658DD}" uniqueName="3" name="avg_high_temp" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{A1AF304D-82AD-4527-B780-73F0BF13822E}" uniqueName="4" name="median_temp" queryTableFieldId="4"/>
@@ -693,7 +2376,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{48A9B814-E8E4-4439-9FA6-BAEABC283712}" name="seasonal_crime" displayName="seasonal_crime" ref="A1:D11" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D11" xr:uid="{48A9B814-E8E4-4439-9FA6-BAEABC283712}"/>
   <tableColumns count="4">
-    <tableColumn id="5" xr3:uid="{1BA2CEF3-EF8F-44CB-9219-EEFC92C250E0}" uniqueName="5" name="location_description" queryTableFieldId="5" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{1BA2CEF3-EF8F-44CB-9219-EEFC92C250E0}" uniqueName="5" name="location_description" queryTableFieldId="5" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{E1BB0EDD-7A7F-4A97-83C6-DE7081B21944}" uniqueName="2" name="location_description_count" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{7D1FB51F-33A5-44D7-9DF4-51C881228398}" uniqueName="3" name="mild_weather" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{A6AFF7AC-7AB5-4C0D-A4B5-45DC99D04751}" uniqueName="4" name="cold_weather" queryTableFieldId="4"/>
@@ -706,7 +2389,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D426E6B7-7E6A-498F-8673-1B60E1B2EBDA}" name="top_10_communities_least" displayName="top_10_communities_least" ref="A1:D11" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D11" xr:uid="{D426E6B7-7E6A-498F-8673-1B60E1B2EBDA}"/>
   <tableColumns count="4">
-    <tableColumn id="5" xr3:uid="{00A00B1E-9532-4845-80ED-72B2DE28ABB2}" uniqueName="5" name="community" queryTableFieldId="5" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00A00B1E-9532-4845-80ED-72B2DE28ABB2}" uniqueName="5" name="community" queryTableFieldId="5" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{5DC39817-37B3-4938-ADA0-AEF35273C1CE}" uniqueName="2" name="population" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{A0D2C5DB-398C-4303-956C-7A8FC39282C2}" uniqueName="3" name="density" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{FC1FB444-9D3E-4CEE-85CF-453CDCACD9D7}" uniqueName="4" name="reported_crimes" queryTableFieldId="4"/>
@@ -719,7 +2402,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{64A1C104-DC1E-4FC7-B87B-20387AF818D8}" name="top_10_communities_most" displayName="top_10_communities_most" ref="A1:D11" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D11" xr:uid="{64A1C104-DC1E-4FC7-B87B-20387AF818D8}"/>
   <tableColumns count="4">
-    <tableColumn id="5" xr3:uid="{C504C3A9-C522-493F-AC78-0158CA68F179}" uniqueName="5" name="community" queryTableFieldId="5" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{C504C3A9-C522-493F-AC78-0158CA68F179}" uniqueName="5" name="community" queryTableFieldId="5" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{413463AF-023C-4751-A3A7-701496446C66}" uniqueName="2" name="population" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{01C7CF50-53CD-427D-832A-902706FEDDF7}" uniqueName="3" name="density" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{181C0646-3415-4694-BF0E-124C3FE8535C}" uniqueName="4" name="reported_crimes" queryTableFieldId="4"/>
@@ -732,7 +2415,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A46E7067-4459-4BC3-93BE-2D1E0153B3EB}" name="top_city_streets" displayName="top_city_streets" ref="A1:B11" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B11" xr:uid="{A46E7067-4459-4BC3-93BE-2D1E0153B3EB}"/>
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{F18F63A7-80D0-40BA-A5E4-E87C689CE657}" uniqueName="3" name="street_name" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{F18F63A7-80D0-40BA-A5E4-E87C689CE657}" uniqueName="3" name="street_name" queryTableFieldId="3" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{E12BC778-ABFA-4346-BF1D-0CE73DA4AF79}" uniqueName="2" name="n_crimes" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -743,7 +2426,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{3CEDD5ED-C7D5-4093-A3B7-286B9ABDF41D}" name="top_crime_month" displayName="top_crime_month" ref="A1:B13" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B13" xr:uid="{3CEDD5ED-C7D5-4093-A3B7-286B9ABDF41D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{26B73A7B-8A59-4A2A-97D1-106C3FF8DCD0}" uniqueName="1" name="month" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{26B73A7B-8A59-4A2A-97D1-106C3FF8DCD0}" uniqueName="1" name="month" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{47D34ADA-03EE-450A-9237-BC56B4176D4B}" uniqueName="2" name="n_crimes" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1071,7 +2754,7 @@
       <c r="A2">
         <v>43</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1106,7 +2789,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>32</v>
       </c>
       <c r="B2">
@@ -1114,7 +2797,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>33</v>
       </c>
       <c r="B3">
@@ -1122,7 +2805,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>34</v>
       </c>
       <c r="B4">
@@ -1130,7 +2813,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>35</v>
       </c>
       <c r="B5">
@@ -1138,7 +2821,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>36</v>
       </c>
       <c r="B6">
@@ -1146,7 +2829,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>37</v>
       </c>
       <c r="B7">
@@ -1154,7 +2837,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>38</v>
       </c>
       <c r="B8">
@@ -1200,7 +2883,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2">
@@ -1214,7 +2897,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3">
@@ -1228,7 +2911,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
@@ -1242,7 +2925,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5">
@@ -1256,7 +2939,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
@@ -1270,7 +2953,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7">
@@ -1284,7 +2967,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8">
@@ -1298,7 +2981,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
@@ -1312,7 +2995,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
@@ -1326,7 +3009,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11">
@@ -1340,7 +3023,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -1354,7 +3037,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13">
@@ -1398,7 +3081,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>52</v>
       </c>
       <c r="B2">
@@ -1406,7 +3089,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>53</v>
       </c>
       <c r="B3">
@@ -1414,7 +3097,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4">
@@ -1422,7 +3105,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>55</v>
       </c>
       <c r="B5">
@@ -1430,7 +3113,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>56</v>
       </c>
       <c r="B6">
@@ -1438,7 +3121,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>57</v>
       </c>
       <c r="B7">
@@ -1446,7 +3129,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>58</v>
       </c>
       <c r="B8">
@@ -1454,7 +3137,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>59</v>
       </c>
       <c r="B9">
@@ -1462,7 +3145,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>60</v>
       </c>
       <c r="B10">
@@ -1470,7 +3153,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>61</v>
       </c>
       <c r="B11">
@@ -1489,7 +3172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E57F053-97EC-4121-9161-8A2187FC139B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -1499,19 +3182,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AC0244-4854-48D5-AFCE-CA30CBB3A325}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1519,18 +3204,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>78.2</v>
       </c>
       <c r="B2">
         <v>21.8</v>
       </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>21.8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>78.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1585,7 +3286,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCD15CC-50FB-4784-854B-06BB83886E30}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1606,7 +3309,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
@@ -1614,7 +3317,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3">
@@ -1625,7 +3328,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4">
@@ -1636,7 +3339,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5">
@@ -1647,7 +3350,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
@@ -1658,7 +3361,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7">
@@ -1669,7 +3372,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8">
@@ -1680,7 +3383,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9">
@@ -1691,7 +3394,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10">
@@ -1702,7 +3405,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11">
@@ -1713,7 +3416,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12">
@@ -1724,7 +3427,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13">
@@ -1773,7 +3476,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>42</v>
       </c>
       <c r="B2">
@@ -1787,7 +3490,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>43</v>
       </c>
       <c r="B3">
@@ -1801,7 +3504,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>44</v>
       </c>
       <c r="B4">
@@ -1815,7 +3518,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>45</v>
       </c>
       <c r="B5">
@@ -1829,7 +3532,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>46</v>
       </c>
       <c r="B6">
@@ -1843,7 +3546,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>47</v>
       </c>
       <c r="B7">
@@ -1857,7 +3560,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>48</v>
       </c>
       <c r="B8">
@@ -1871,7 +3574,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>49</v>
       </c>
       <c r="B9">
@@ -1885,7 +3588,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>50</v>
       </c>
       <c r="B10">
@@ -1899,7 +3602,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>51</v>
       </c>
       <c r="B11">
@@ -1951,7 +3654,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>78</v>
       </c>
       <c r="B2">
@@ -1965,7 +3668,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>79</v>
       </c>
       <c r="B3">
@@ -1979,7 +3682,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>80</v>
       </c>
       <c r="B4">
@@ -1993,7 +3696,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>81</v>
       </c>
       <c r="B5">
@@ -2007,7 +3710,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>82</v>
       </c>
       <c r="B6">
@@ -2021,7 +3724,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>83</v>
       </c>
       <c r="B7">
@@ -2035,7 +3738,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>84</v>
       </c>
       <c r="B8">
@@ -2049,7 +3752,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>85</v>
       </c>
       <c r="B9">
@@ -2063,7 +3766,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>86</v>
       </c>
       <c r="B10">
@@ -2077,7 +3780,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>87</v>
       </c>
       <c r="B11">
@@ -2129,7 +3832,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>68</v>
       </c>
       <c r="B2">
@@ -2143,7 +3846,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>69</v>
       </c>
       <c r="B3">
@@ -2157,7 +3860,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>70</v>
       </c>
       <c r="B4">
@@ -2171,7 +3874,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>71</v>
       </c>
       <c r="B5">
@@ -2185,7 +3888,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>72</v>
       </c>
       <c r="B6">
@@ -2199,7 +3902,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>73</v>
       </c>
       <c r="B7">
@@ -2213,7 +3916,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>74</v>
       </c>
       <c r="B8">
@@ -2227,7 +3930,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>75</v>
       </c>
       <c r="B9">
@@ -2241,7 +3944,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>76</v>
       </c>
       <c r="B10">
@@ -2255,7 +3958,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>77</v>
       </c>
       <c r="B11">
@@ -2299,7 +4002,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>56</v>
       </c>
       <c r="B2">
@@ -2307,7 +4010,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>62</v>
       </c>
       <c r="B3">
@@ -2315,7 +4018,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>63</v>
       </c>
       <c r="B4">
@@ -2323,7 +4026,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>64</v>
       </c>
       <c r="B5">
@@ -2331,7 +4034,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>65</v>
       </c>
       <c r="B6">
@@ -2339,7 +4042,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>66</v>
       </c>
       <c r="B7">
@@ -2347,7 +4050,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>60</v>
       </c>
       <c r="B8">
@@ -2355,7 +4058,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>61</v>
       </c>
       <c r="B9">
@@ -2363,7 +4066,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>67</v>
       </c>
       <c r="B10">
@@ -2371,7 +4074,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>53</v>
       </c>
       <c r="B11">
@@ -2409,7 +4112,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2">
@@ -2417,7 +4120,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3">
@@ -2425,7 +4128,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4">
@@ -2433,7 +4136,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5">
@@ -2441,7 +4144,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6">
@@ -2449,7 +4152,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
@@ -2457,7 +4160,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8">
@@ -2465,7 +4168,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
@@ -2473,7 +4176,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
@@ -2481,7 +4184,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
@@ -2489,7 +4192,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12">
@@ -2497,7 +4200,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13">

</xml_diff>

<commit_message>
Adding monthly temp and homicide count chart
</commit_message>
<xml_diff>
--- a/excel/sql_query_output.xlsx
+++ b/excel/sql_query_output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime\Desktop\git-repo\chicago_crime_and_weather_2021\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB70177-A0FB-42AA-9483-1532E275945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC23673-3D2C-478F-9402-781ED28E0B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-705" windowWidth="28110" windowHeight="16440" activeTab="3" xr2:uid="{CE6839DA-4336-434C-A3C6-5CF43E49803F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="6" activeTab="10" xr2:uid="{CE6839DA-4336-434C-A3C6-5CF43E49803F}"/>
   </bookViews>
   <sheets>
     <sheet name="consecutive_homicide" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId14"/>
+    <pivotCache cacheId="0" r:id="rId14"/>
+    <pivotCache cacheId="3" r:id="rId15"/>
+    <pivotCache cacheId="6" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -106,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="95">
   <si>
     <t>most_consecutive_days</t>
   </si>
@@ -376,6 +378,21 @@
   </si>
   <si>
     <t>Sum of non_domestic_violence</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of n_crimes</t>
+  </si>
+  <si>
+    <t>Sum of n_homicides</t>
+  </si>
+  <si>
+    <t>Sum of avg_high_temp</t>
   </si>
 </sst>
 </file>
@@ -411,14 +428,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -838,6 +868,16 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-82E7-4BE7-A3BC-3EED7278D295}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
@@ -1262,7 +1302,880 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[sql_query_output.xlsx]top_month_homicide!PivotTable2</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:gradFill>
+            <a:gsLst>
+              <a:gs pos="90000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="1000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="45000"/>
+                  <a:lumOff val="55000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+          </a:gradFill>
+          <a:ln>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="5000"/>
+                    <a:lumOff val="95000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="97000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="45000"/>
+                    <a:lumOff val="55000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+            </a:gradFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="inBase"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>top_month_homicide!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum of n_homicides</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="90000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="5000"/>
+                    <a:lumOff val="95000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="1000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="45000"/>
+                    <a:lumOff val="55000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+            </a:gradFill>
+            <a:ln>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="5000"/>
+                      <a:lumOff val="95000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="97000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="45000"/>
+                      <a:lumOff val="55000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="1"/>
+              </a:gradFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>top_month_homicide!$F$3:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>January  </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March    </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April    </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May      </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June     </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July     </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August   </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October  </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November </c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>top_month_homicide!$G$3:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E2F4-4FEB-A021-32AB6FF14DAD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="78"/>
+        <c:axId val="895105888"/>
+        <c:axId val="895095488"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>top_month_homicide!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum of avg_high_temp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>top_month_homicide!$F$3:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>January  </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March    </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April    </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May      </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June     </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July     </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August   </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October  </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November </c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>top_month_homicide!$H$3:$H$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>34.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>73.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E2F4-4FEB-A021-32AB6FF14DAD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="498311888"/>
+        <c:axId val="498308976"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="498311888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="498308976"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="498308976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="#,##0;\-#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="498311888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="895095488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="895105888"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="895105888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="895095488"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1452,6 +2365,522 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2013,7 +3442,7 @@
                   </a:schemeClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t> crimes where some form of domestic violence.</a:t>
+              <a:t> crimes where a result of domestic violence.</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1200">
               <a:solidFill>
@@ -2028,6 +3457,356 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7994AFA0-14CD-6E91-B566-5ED39B91082D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4333875" y="3067050"/>
+          <a:ext cx="7010400" cy="3314700"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 4023"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>165351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D02C67A9-205D-09DD-500F-A7EA7BDDA87E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36D0F4BB-3FB7-32AD-198C-DA99FA57C2DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4362450" y="3143250"/>
+          <a:ext cx="1828800" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>February was the coldest month of the year with a median</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t> temperature of 26</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>° and had 38 reported homicides.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+            <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>As the weather gets milder, we see a sharp increase</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t> in all crimes during the late Spring through the early Fall.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76197</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>704848</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66672</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Arrow: Left-Up 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2D36A25-F03E-94C7-4AFD-F53F5FBC198D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="7000874" y="3695697"/>
+          <a:ext cx="1790699" cy="1133475"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftUpArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 9874"/>
+            <a:gd name="adj2" fmla="val 10294"/>
+            <a:gd name="adj3" fmla="val 14075"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2505075" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE3A17CA-9037-841C-DD86-140C37D75DAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8696325" y="3228974"/>
+          <a:ext cx="2505075" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The number</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> of Homicides </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>increased</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> almost 200% between February and July</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2052,6 +3831,80 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jaime" refreshedDate="44934.262888310186" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="12" xr:uid="{AC67A58B-3270-4A07-8E7E-7922CC63D8D5}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="top_crime_month"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="month" numFmtId="0">
+      <sharedItems count="12">
+        <s v="October  "/>
+        <s v="September"/>
+        <s v="July     "/>
+        <s v="June     "/>
+        <s v="August   "/>
+        <s v="May      "/>
+        <s v="November "/>
+        <s v="January  "/>
+        <s v="March    "/>
+        <s v="April    "/>
+        <s v="December "/>
+        <s v="February "/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="n_crimes" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12888" maxValue="19018"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jaime" refreshedDate="44934.264353587962" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="12" xr:uid="{C714AC48-FC58-4BAD-8F81-4C5E17ACB6F2}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="top_month_homicide"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="month" numFmtId="0">
+      <sharedItems count="12">
+        <s v="July     "/>
+        <s v="September"/>
+        <s v="June     "/>
+        <s v="August   "/>
+        <s v="May      "/>
+        <s v="October  "/>
+        <s v="November "/>
+        <s v="January  "/>
+        <s v="April    "/>
+        <s v="December "/>
+        <s v="March    "/>
+        <s v="February "/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="n_homicides" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="38" maxValue="112"/>
+    </cacheField>
+    <cacheField name="avg_high_temp" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="27" maxValue="85.3"/>
+    </cacheField>
+    <cacheField name="median_temp" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="26" maxValue="85"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
@@ -2061,8 +3914,138 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="12">
+  <r>
+    <x v="0"/>
+    <n v="19018"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="18987"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="18966"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="18566"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="18255"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="17539"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="16974"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="16038"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="15742"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="15305"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="14258"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="12888"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="12">
+  <r>
+    <x v="0"/>
+    <n v="112"/>
+    <n v="82.6"/>
+    <n v="82"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="89"/>
+    <n v="80.8"/>
+    <n v="82"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="85"/>
+    <n v="83.5"/>
+    <n v="82"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="81"/>
+    <n v="85.3"/>
+    <n v="85"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="66"/>
+    <n v="73.900000000000006"/>
+    <n v="75.5"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="64"/>
+    <n v="67.900000000000006"/>
+    <n v="71"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="62"/>
+    <n v="50.6"/>
+    <n v="51"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="55"/>
+    <n v="34.1"/>
+    <n v="34"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="54"/>
+    <n v="65.099999999999994"/>
+    <n v="62"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="52"/>
+    <n v="48.6"/>
+    <n v="49"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="45"/>
+    <n v="54.7"/>
+    <n v="52"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="38"/>
+    <n v="27"/>
+    <n v="26"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7400F035-ADCB-442E-9D3B-CA40FF32DF26}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7400F035-ADCB-442E-9D3B-CA40FF32DF26}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D2:E3" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0"/>
@@ -2119,6 +4102,207 @@
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5A4A6DBA-0D8C-4A4F-8EF1-B3A800D707D7}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="E1:F14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="1"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of n_crimes" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{898CC059-EB55-48E2-9B84-1F77F30BA893}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="F2:H15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="7"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="8"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of n_homicides" fld="1" baseField="0" baseItem="0"/>
+    <dataField name="Sum of avg_high_temp" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -2297,7 +4481,7 @@
   <autoFilter ref="A1:B2" xr:uid="{438FFE49-9EF8-4757-B5BD-49D36E45BA14}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3548F753-79BE-40DF-8FC3-45BF9220E40F}" uniqueName="1" name="most_consecutive_days" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{28F26E73-2DA6-4049-B3AE-6BA81F6B97D7}" uniqueName="2" name="time_frame" queryTableFieldId="2" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{28F26E73-2DA6-4049-B3AE-6BA81F6B97D7}" uniqueName="2" name="time_frame" queryTableFieldId="2" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2307,7 +4491,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E3BC32D3-E9CB-4FB9-9F98-7D59A879005B}" name="top_crime_weekday" displayName="top_crime_weekday" ref="A1:B8" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B8" xr:uid="{E3BC32D3-E9CB-4FB9-9F98-7D59A879005B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{AD5E170E-73C4-454E-82B1-7DA81A6EFCD6}" uniqueName="1" name="day_of_week" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{AD5E170E-73C4-454E-82B1-7DA81A6EFCD6}" uniqueName="1" name="day_of_week" queryTableFieldId="1" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{C9E87FF3-75EF-4377-85FE-178D46DAA5F2}" uniqueName="2" name="n_crimes" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2318,7 +4502,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0D92DAAA-F6FE-4B2E-A008-6757307FA6F8}" name="top_month_homicide" displayName="top_month_homicide" ref="A1:D13" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D13" xr:uid="{0D92DAAA-F6FE-4B2E-A008-6757307FA6F8}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{64A4C862-9E4C-410F-943B-F731E46517EB}" uniqueName="1" name="month" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{64A4C862-9E4C-410F-943B-F731E46517EB}" uniqueName="1" name="month" queryTableFieldId="1" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{2BE5E1AF-87B9-46BA-8E84-007DB57234B9}" uniqueName="2" name="n_homicides" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{4A4D9BAB-E3DB-4685-939B-77B2472658DD}" uniqueName="3" name="avg_high_temp" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{A1AF304D-82AD-4527-B780-73F0BF13822E}" uniqueName="4" name="median_temp" queryTableFieldId="4"/>
@@ -2331,7 +4515,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{A3C30479-66F2-4912-8EB1-49B588FE4AF8}" name="top_streets_homicide" displayName="top_streets_homicide" ref="A1:B11" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B11" xr:uid="{A3C30479-66F2-4912-8EB1-49B588FE4AF8}"/>
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{2856F69C-56BF-4EC1-ABBD-9A06FCFD5DD1}" uniqueName="3" name="street_name" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{2856F69C-56BF-4EC1-ABBD-9A06FCFD5DD1}" uniqueName="3" name="street_name" queryTableFieldId="3" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{495CE841-A21A-4EF3-AC9E-A457CE405521}" uniqueName="2" name="n_homicides" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2364,7 +4548,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4363CAB7-AE5A-46E5-B78B-ECA09F99371A}" name="month_to_month" displayName="month_to_month" ref="A1:C13" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C13" xr:uid="{4363CAB7-AE5A-46E5-B78B-ECA09F99371A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BD4E80E4-2C43-4ADC-997A-5BA3D7ED6959}" uniqueName="1" name="crime_month" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{BD4E80E4-2C43-4ADC-997A-5BA3D7ED6959}" uniqueName="1" name="crime_month" queryTableFieldId="1" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{286AAAD4-1553-496E-B1F0-70C8BDC24D68}" uniqueName="2" name="n_crimes" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{536637E0-664B-41DA-BAAB-EDC4E0294B8B}" uniqueName="3" name="month_to_month" queryTableFieldId="3"/>
   </tableColumns>
@@ -2376,7 +4560,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{48A9B814-E8E4-4439-9FA6-BAEABC283712}" name="seasonal_crime" displayName="seasonal_crime" ref="A1:D11" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D11" xr:uid="{48A9B814-E8E4-4439-9FA6-BAEABC283712}"/>
   <tableColumns count="4">
-    <tableColumn id="5" xr3:uid="{1BA2CEF3-EF8F-44CB-9219-EEFC92C250E0}" uniqueName="5" name="location_description" queryTableFieldId="5" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{1BA2CEF3-EF8F-44CB-9219-EEFC92C250E0}" uniqueName="5" name="location_description" queryTableFieldId="5" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{E1BB0EDD-7A7F-4A97-83C6-DE7081B21944}" uniqueName="2" name="location_description_count" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{7D1FB51F-33A5-44D7-9DF4-51C881228398}" uniqueName="3" name="mild_weather" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{A6AFF7AC-7AB5-4C0D-A4B5-45DC99D04751}" uniqueName="4" name="cold_weather" queryTableFieldId="4"/>
@@ -2389,7 +4573,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D426E6B7-7E6A-498F-8673-1B60E1B2EBDA}" name="top_10_communities_least" displayName="top_10_communities_least" ref="A1:D11" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D11" xr:uid="{D426E6B7-7E6A-498F-8673-1B60E1B2EBDA}"/>
   <tableColumns count="4">
-    <tableColumn id="5" xr3:uid="{00A00B1E-9532-4845-80ED-72B2DE28ABB2}" uniqueName="5" name="community" queryTableFieldId="5" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00A00B1E-9532-4845-80ED-72B2DE28ABB2}" uniqueName="5" name="community" queryTableFieldId="5" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{5DC39817-37B3-4938-ADA0-AEF35273C1CE}" uniqueName="2" name="population" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{A0D2C5DB-398C-4303-956C-7A8FC39282C2}" uniqueName="3" name="density" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{FC1FB444-9D3E-4CEE-85CF-453CDCACD9D7}" uniqueName="4" name="reported_crimes" queryTableFieldId="4"/>
@@ -2402,7 +4586,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{64A1C104-DC1E-4FC7-B87B-20387AF818D8}" name="top_10_communities_most" displayName="top_10_communities_most" ref="A1:D11" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D11" xr:uid="{64A1C104-DC1E-4FC7-B87B-20387AF818D8}"/>
   <tableColumns count="4">
-    <tableColumn id="5" xr3:uid="{C504C3A9-C522-493F-AC78-0158CA68F179}" uniqueName="5" name="community" queryTableFieldId="5" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{C504C3A9-C522-493F-AC78-0158CA68F179}" uniqueName="5" name="community" queryTableFieldId="5" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{413463AF-023C-4751-A3A7-701496446C66}" uniqueName="2" name="population" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{01C7CF50-53CD-427D-832A-902706FEDDF7}" uniqueName="3" name="density" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{181C0646-3415-4694-BF0E-124C3FE8535C}" uniqueName="4" name="reported_crimes" queryTableFieldId="4"/>
@@ -2415,7 +4599,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A46E7067-4459-4BC3-93BE-2D1E0153B3EB}" name="top_city_streets" displayName="top_city_streets" ref="A1:B11" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B11" xr:uid="{A46E7067-4459-4BC3-93BE-2D1E0153B3EB}"/>
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{F18F63A7-80D0-40BA-A5E4-E87C689CE657}" uniqueName="3" name="street_name" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F18F63A7-80D0-40BA-A5E4-E87C689CE657}" uniqueName="3" name="street_name" queryTableFieldId="3" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{E12BC778-ABFA-4346-BF1D-0CE73DA4AF79}" uniqueName="2" name="n_crimes" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2426,7 +4610,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{3CEDD5ED-C7D5-4093-A3B7-286B9ABDF41D}" name="top_crime_month" displayName="top_crime_month" ref="A1:B13" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B13" xr:uid="{3CEDD5ED-C7D5-4093-A3B7-286B9ABDF41D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{26B73A7B-8A59-4A2A-97D1-106C3FF8DCD0}" uniqueName="1" name="month" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{26B73A7B-8A59-4A2A-97D1-106C3FF8DCD0}" uniqueName="1" name="month" queryTableFieldId="1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{47D34ADA-03EE-450A-9237-BC56B4176D4B}" uniqueName="2" name="n_crimes" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2854,10 +5038,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338E6105-BFC5-4570-A024-BCCE2469B950}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2866,9 +5050,13 @@
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2882,7 +5070,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2895,8 +5083,17 @@
       <c r="D2">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2909,8 +5106,17 @@
       <c r="D3">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3">
+        <v>55</v>
+      </c>
+      <c r="H3" s="3">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2923,8 +5129,17 @@
       <c r="D4">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3">
+        <v>38</v>
+      </c>
+      <c r="H4" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2937,8 +5152,17 @@
       <c r="D5">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3">
+        <v>45</v>
+      </c>
+      <c r="H5" s="3">
+        <v>54.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2951,8 +5175,17 @@
       <c r="D6">
         <v>75.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3">
+        <v>54</v>
+      </c>
+      <c r="H6" s="3">
+        <v>65.099999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2965,8 +5198,17 @@
       <c r="D7">
         <v>71</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3">
+        <v>66</v>
+      </c>
+      <c r="H7" s="3">
+        <v>73.900000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2979,8 +5221,17 @@
       <c r="D8">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="3">
+        <v>85</v>
+      </c>
+      <c r="H8" s="3">
+        <v>83.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2993,8 +5244,17 @@
       <c r="D9">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="3">
+        <v>112</v>
+      </c>
+      <c r="H9" s="3">
+        <v>82.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3007,8 +5267,17 @@
       <c r="D10">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="3">
+        <v>81</v>
+      </c>
+      <c r="H10" s="3">
+        <v>85.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3021,8 +5290,17 @@
       <c r="D11">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="3">
+        <v>89</v>
+      </c>
+      <c r="H11" s="3">
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3035,8 +5313,17 @@
       <c r="D12">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="3">
+        <v>64</v>
+      </c>
+      <c r="H12" s="3">
+        <v>67.900000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3049,11 +5336,43 @@
       <c r="D13">
         <v>26</v>
       </c>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="3">
+        <v>62</v>
+      </c>
+      <c r="H13" s="3">
+        <v>50.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="3">
+        <v>52</v>
+      </c>
+      <c r="H14" s="3">
+        <v>48.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="3">
+        <v>803</v>
+      </c>
+      <c r="H15" s="3">
+        <v>754.1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3185,7 +5504,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3219,10 +5538,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D3" s="1">
+      <c r="D3">
         <v>21.8</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>78.2</v>
       </c>
     </row>
@@ -3286,8 +5605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCD15CC-50FB-4784-854B-06BB83886E30}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4091,126 +6410,214 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3437103E-2392-4D11-BAF6-74069E931570}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2">
         <v>19018</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3">
+        <v>18987</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3">
         <v>18987</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3">
+        <v>15305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4">
         <v>18966</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3">
+        <v>18255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5">
         <v>18566</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3">
+        <v>14258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6">
         <v>18255</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3">
+        <v>12888</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
         <v>17539</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3">
+        <v>16038</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8">
         <v>16974</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="3">
+        <v>18966</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>16038</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="3">
+        <v>18566</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
         <v>15742</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3">
+        <v>15742</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
         <v>15305</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="3">
+        <v>17539</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12">
         <v>14258</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="3">
+        <v>16974</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13">
         <v>12888</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="3">
+        <v>19018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="3">
+        <v>202536</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Adding visualization to mild vs cold query
</commit_message>
<xml_diff>
--- a/excel/sql_query_output.xlsx
+++ b/excel/sql_query_output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime\Desktop\git-repo\chicago_crime_and_weather_2021\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A03C8BC-034F-44B4-9CAB-D50696A93B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C79C2A-EDDB-4044-BA8A-B7F79C799C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{CE6839DA-4336-434C-A3C6-5CF43E49803F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="4" activeTab="8" xr2:uid="{CE6839DA-4336-434C-A3C6-5CF43E49803F}"/>
   </bookViews>
   <sheets>
     <sheet name="consecutive_homicide" sheetId="2" r:id="rId1"/>
@@ -314,66 +314,6 @@
     <t xml:space="preserve"> Kedzie Ave.</t>
   </si>
   <si>
-    <t>Austin.</t>
-  </si>
-  <si>
-    <t>Near North Side.</t>
-  </si>
-  <si>
-    <t>South Shore.</t>
-  </si>
-  <si>
-    <t>Near West Side.</t>
-  </si>
-  <si>
-    <t>North Lawndale.</t>
-  </si>
-  <si>
-    <t>Auburn Gresham.</t>
-  </si>
-  <si>
-    <t>Humboldt Park.</t>
-  </si>
-  <si>
-    <t>Greater Grand Crossing.</t>
-  </si>
-  <si>
-    <t>West Town.</t>
-  </si>
-  <si>
-    <t>Loop.</t>
-  </si>
-  <si>
-    <t>Edison Park.</t>
-  </si>
-  <si>
-    <t>Burnside.</t>
-  </si>
-  <si>
-    <t>Forest Glen.</t>
-  </si>
-  <si>
-    <t>Mount Greenwood.</t>
-  </si>
-  <si>
-    <t>Montclare.</t>
-  </si>
-  <si>
-    <t>Fuller Park.</t>
-  </si>
-  <si>
-    <t>Oakland.</t>
-  </si>
-  <si>
-    <t>Hegewisch.</t>
-  </si>
-  <si>
-    <t>Archer Heights.</t>
-  </si>
-  <si>
-    <t>North Park.</t>
-  </si>
-  <si>
     <t>Sum of domestic_violence</t>
   </si>
   <si>
@@ -393,6 +333,66 @@
   </si>
   <si>
     <t>Sum of avg_high_temp</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Near North Side</t>
+  </si>
+  <si>
+    <t>South Shore</t>
+  </si>
+  <si>
+    <t>Near West Side</t>
+  </si>
+  <si>
+    <t>North Lawndale</t>
+  </si>
+  <si>
+    <t>Auburn Gresham</t>
+  </si>
+  <si>
+    <t>Humboldt Park</t>
+  </si>
+  <si>
+    <t>Greater Grand Crossing</t>
+  </si>
+  <si>
+    <t>West Town</t>
+  </si>
+  <si>
+    <t>Loop</t>
+  </si>
+  <si>
+    <t>Edison Park</t>
+  </si>
+  <si>
+    <t>Burnside</t>
+  </si>
+  <si>
+    <t>Forest Glen</t>
+  </si>
+  <si>
+    <t>Mount Greenwood</t>
+  </si>
+  <si>
+    <t>Montclare</t>
+  </si>
+  <si>
+    <t>Fuller Park</t>
+  </si>
+  <si>
+    <t>Oakland</t>
+  </si>
+  <si>
+    <t>Hegewisch</t>
+  </si>
+  <si>
+    <t>Archer Heights</t>
+  </si>
+  <si>
+    <t>North Park</t>
   </si>
 </sst>
 </file>
@@ -434,13 +434,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1309,6 +1311,412 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[sql_query_output.xlsx]top_crime_month!PivotTable1</c:name>
+    <c:fmtId val="1"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="22000">
+                  <a:srgbClr val="C00000"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="40000"/>
+                    <a:lumOff val="60000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="0" scaled="0"/>
+            </a:gradFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>top_crime_month!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="22000">
+                    <a:srgbClr val="C00000"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="40000"/>
+                      <a:lumOff val="60000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="0" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>top_crime_month!$E$2:$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>October  </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>July     </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>June     </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>August   </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>May      </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>November </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>January  </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>March    </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>April    </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>December </c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>February </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>top_crime_month!$F$2:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>19018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18987</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18966</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18566</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17539</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16974</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16038</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15742</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15305</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14258</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12888</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5171-4CC8-AE56-A82FA64F1FB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1913673264"/>
+        <c:axId val="1913671600"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1913673264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1913671600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1913671600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1913673264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2225,6 +2633,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2729,6 +3177,511 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3471,6 +4424,261 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="Group 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AB993DE-3599-6515-CC01-C3C9203DA172}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3000375" y="3324225"/>
+          <a:ext cx="4686299" cy="2476500"/>
+          <a:chOff x="8353425" y="3314700"/>
+          <a:chExt cx="4686299" cy="2476500"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F051E16-EF22-780A-5D23-08672AF2A1C8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8353425" y="3314700"/>
+            <a:ext cx="4686299" cy="2476500"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 2963"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="2" name="Chart 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0E3BC2C-9BE5-9E92-7812-BC523F302554}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="8420100" y="3400425"/>
+          <a:ext cx="4533900" cy="2305049"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Rectangle: Rounded Corners 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D01A753E-6D7B-A796-12E7-F130EA8AC149}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10220325" y="4362451"/>
+            <a:ext cx="2581275" cy="495300"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 6079"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="TextBox 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA5BB074-5F56-99C1-8DA7-EEB7C8B4B58C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10229850" y="4381499"/>
+            <a:ext cx="2562226" cy="448641"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>The highest</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> amount of reported crimes occured during the mild weather months.  </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4130,23 +5338,23 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5A4A6DBA-0D8C-4A4F-8EF1-B3A800D707D7}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5A4A6DBA-0D8C-4A4F-8EF1-B3A800D707D7}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="E1:F14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
       <items count="13">
+        <item x="0"/>
         <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
         <item x="9"/>
-        <item x="4"/>
         <item x="10"/>
         <item x="11"/>
-        <item x="7"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="8"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -4202,6 +5410,17 @@
   <dataFields count="1">
     <dataField name="Sum of n_crimes" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -5094,13 +6313,13 @@
         <v>82</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -5369,7 +6588,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F15" s="2" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="G15">
         <v>803</v>
@@ -5733,7 +6952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AC0244-4854-48D5-AFCE-CA30CBB3A325}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -5761,10 +6980,10 @@
         <v>21.8</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -6229,7 +7448,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6256,7 +7475,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B2">
         <v>11525</v>
@@ -6270,7 +7489,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B3">
         <v>2527</v>
@@ -6284,7 +7503,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B4">
         <v>19596</v>
@@ -6298,7 +7517,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B5">
         <v>18628</v>
@@ -6312,7 +7531,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B6">
         <v>14401</v>
@@ -6326,7 +7545,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B7">
         <v>2567</v>
@@ -6340,7 +7559,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B8">
         <v>6799</v>
@@ -6354,7 +7573,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B9">
         <v>10027</v>
@@ -6368,7 +7587,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B10">
         <v>14196</v>
@@ -6382,7 +7601,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B11">
         <v>17559</v>
@@ -6407,7 +7626,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6434,7 +7653,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B2">
         <v>96557</v>
@@ -6448,7 +7667,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B3">
         <v>105481</v>
@@ -6462,7 +7681,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B4">
         <v>53971</v>
@@ -6476,7 +7695,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B5">
         <v>67881</v>
@@ -6490,7 +7709,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B6">
         <v>34794</v>
@@ -6504,7 +7723,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B7">
         <v>44878</v>
@@ -6518,7 +7737,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B8">
         <v>54165</v>
@@ -6532,7 +7751,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B9">
         <v>31471</v>
@@ -6546,7 +7765,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B10">
         <v>87781</v>
@@ -6560,7 +7779,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B11">
         <v>42298</v>
@@ -6692,10 +7911,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3437103E-2392-4D11-BAF6-74069E931570}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6704,6 +7923,18 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6714,10 +7945,10 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -6728,10 +7959,10 @@
         <v>19018</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>18987</v>
+        <v>18</v>
+      </c>
+      <c r="F2" s="4">
+        <v>19018</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -6742,10 +7973,10 @@
         <v>18987</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>15305</v>
+        <v>17</v>
+      </c>
+      <c r="F3" s="4">
+        <v>18987</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6756,10 +7987,10 @@
         <v>18966</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4">
-        <v>18255</v>
+        <v>15</v>
+      </c>
+      <c r="F4" s="4">
+        <v>18966</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6770,10 +8001,10 @@
         <v>18566</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5">
-        <v>14258</v>
+        <v>14</v>
+      </c>
+      <c r="F5" s="4">
+        <v>18566</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6784,10 +8015,10 @@
         <v>18255</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>12888</v>
+        <v>16</v>
+      </c>
+      <c r="F6" s="4">
+        <v>18255</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -6798,10 +8029,10 @@
         <v>17539</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7">
-        <v>16038</v>
+        <v>13</v>
+      </c>
+      <c r="F7" s="4">
+        <v>17539</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -6812,10 +8043,10 @@
         <v>16974</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8">
-        <v>18966</v>
+        <v>19</v>
+      </c>
+      <c r="F8" s="4">
+        <v>16974</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -6826,10 +8057,10 @@
         <v>16038</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9">
-        <v>18566</v>
+        <v>9</v>
+      </c>
+      <c r="F9" s="4">
+        <v>16038</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -6842,7 +8073,7 @@
       <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="4">
         <v>15742</v>
       </c>
     </row>
@@ -6854,10 +8085,10 @@
         <v>15305</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11">
-        <v>17539</v>
+        <v>12</v>
+      </c>
+      <c r="F11" s="4">
+        <v>15305</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -6868,10 +8099,10 @@
         <v>14258</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12">
-        <v>16974</v>
+        <v>20</v>
+      </c>
+      <c r="F12" s="4">
+        <v>14258</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -6882,24 +8113,340 @@
         <v>12888</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13">
-        <v>19018</v>
+        <v>10</v>
+      </c>
+      <c r="F13" s="4">
+        <v>12888</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F14">
+        <v>71</v>
+      </c>
+      <c r="F14" s="4">
         <v>202536</v>
       </c>
+    </row>
+    <row r="17" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+    </row>
+    <row r="18" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+    </row>
+    <row r="19" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+    </row>
+    <row r="20" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+    </row>
+    <row r="21" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+    </row>
+    <row r="22" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+    </row>
+    <row r="23" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+    </row>
+    <row r="24" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+    </row>
+    <row r="25" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+    </row>
+    <row r="26" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+    </row>
+    <row r="27" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+    </row>
+    <row r="28" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+    </row>
+    <row r="29" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+    </row>
+    <row r="30" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+    </row>
+    <row r="31" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+    </row>
+    <row r="32" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+    </row>
+    <row r="33" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Adding bar chart for day of the week totals to excel file
</commit_message>
<xml_diff>
--- a/excel/sql_query_output.xlsx
+++ b/excel/sql_query_output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime\Desktop\git-repo\chicago_crime_and_weather_2021\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C79C2A-EDDB-4044-BA8A-B7F79C799C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2A005E7-00F5-43A9-A368-4C94B94A4BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="4" activeTab="8" xr2:uid="{CE6839DA-4336-434C-A3C6-5CF43E49803F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="6" activeTab="9" xr2:uid="{CE6839DA-4336-434C-A3C6-5CF43E49803F}"/>
   </bookViews>
   <sheets>
     <sheet name="consecutive_homicide" sheetId="2" r:id="rId1"/>
@@ -46,6 +46,7 @@
     <pivotCache cacheId="0" r:id="rId14"/>
     <pivotCache cacheId="1" r:id="rId15"/>
     <pivotCache cacheId="2" r:id="rId16"/>
+    <pivotCache cacheId="5" r:id="rId17"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -108,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="95">
   <si>
     <t>most_consecutive_days</t>
   </si>
@@ -434,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -442,7 +443,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1392,7 +1392,6 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1550,7 +1549,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1717,6 +1715,589 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[sql_query_output.xlsx]top_crime_weekday!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:gradFill>
+            <a:gsLst>
+              <a:gs pos="8000">
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:gradFill>
+            <a:gsLst>
+              <a:gs pos="25000">
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="94000">
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:gradFill>
+            <a:gsLst>
+              <a:gs pos="8000">
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>top_crime_weekday!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="8000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="1"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0BFF-4E77-B00F-6C46870BAF24}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="8000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="1"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-0BFF-4E77-B00F-6C46870BAF24}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="25000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="94000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="1"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-0BFF-4E77-B00F-6C46870BAF24}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>top_crime_weekday!$D$3:$D$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Sunday   </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Saturday </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Friday   </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thursday </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tuesday  </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Monday   </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>top_crime_weekday!$E$3:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>29569</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29841</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29829</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27825</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28143</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29194</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0BFF-4E77-B00F-6C46870BAF24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="85"/>
+        <c:overlap val="-13"/>
+        <c:axId val="1826998991"/>
+        <c:axId val="1826995247"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1826998991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1826995247"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1826995247"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1826998991"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2673,6 +3254,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3682,6 +4303,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4683,6 +5807,422 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="27" name="Group 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63CD4CB2-BF25-CE0A-F1A9-CE73228D5067}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3457575" y="2790824"/>
+          <a:ext cx="6610351" cy="2619375"/>
+          <a:chOff x="3171825" y="4438649"/>
+          <a:chExt cx="6610351" cy="2619375"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1FDBDFA-08FA-1947-FDEA-AE144C936676}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3171825" y="4533900"/>
+            <a:ext cx="6305550" cy="2524124"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 4305"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="2" name="Chart 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C17F229-A57D-CB05-55B8-B520D0237A52}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="3228974" y="4438649"/>
+          <a:ext cx="4991101" cy="2562225"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="Rectangle: Rounded Corners 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D61C0A11-ADE5-C7D7-A253-2086FEC9707B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6981825" y="5029200"/>
+            <a:ext cx="2438399" cy="714375"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 10000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="TextBox 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4860A6F5-530C-7D77-FAD2-6C79AD836F29}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6991350" y="5153025"/>
+            <a:ext cx="2790826" cy="542925"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Reported</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> crimes increased up to 7% during the weekends</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="21" name="Straight Connector 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4886B64A-5A0A-9C6B-59D2-D12D2300A537}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8582025" y="5705475"/>
+            <a:ext cx="0" cy="1000125"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{886BBF20-DB14-045E-F021-065EE17F7CFE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="7924800" y="6029325"/>
+            <a:ext cx="657225" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D9C4E25-DBC1-43E2-ABC4-12CCB36426AE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="7924800" y="6362700"/>
+            <a:ext cx="657225" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC8911FC-607B-496D-817D-F41F5DC344C8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="7581900" y="6705600"/>
+            <a:ext cx="1000125" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -5123,6 +6663,35 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jaime" refreshedDate="44936.841619791667" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="7" xr:uid="{F54CC4B2-8CC2-4017-B997-294F5DAED72A}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="top_crime_weekday"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="day_of_week" numFmtId="0">
+      <sharedItems count="7">
+        <s v="Saturday "/>
+        <s v="Friday   "/>
+        <s v="Sunday   "/>
+        <s v="Monday   "/>
+        <s v="Wednesday"/>
+        <s v="Tuesday  "/>
+        <s v="Thursday "/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="n_crimes" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="27825" maxValue="29841"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
@@ -5258,6 +6827,39 @@
     <n v="38"/>
     <n v="27"/>
     <n v="26"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="7">
+  <r>
+    <x v="0"/>
+    <n v="29841"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="29829"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="29569"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="29194"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="28143"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="28135"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="27825"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -5434,6 +7036,118 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{26D5272B-BB1B-4B4D-BF77-AE571D1AD95F}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="D2:E10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of n_crimes" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{898CC059-EB55-48E2-9B84-1F77F30BA893}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="F2:H15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
@@ -6181,19 +7895,21 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E22186-5F97-42B1-88D0-FEB851F60869}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -6201,66 +7917,346 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
       <c r="B2">
         <v>29841</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
       <c r="B3">
         <v>29829</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="4">
+        <v>29569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
       <c r="B4">
         <v>29569</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="4">
+        <v>29841</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
       <c r="B5">
         <v>29194</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="4">
+        <v>29829</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
       <c r="B6">
         <v>28143</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="4">
+        <v>27825</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
       <c r="B7">
         <v>28135</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="4">
+        <v>28143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
       <c r="B8">
         <v>27825</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="4">
+        <v>28135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4">
+        <v>29194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="4">
+        <v>202536</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7911,10 +9907,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3437103E-2392-4D11-BAF6-74069E931570}">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7961,7 +9957,7 @@
       <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2">
         <v>19018</v>
       </c>
     </row>
@@ -7975,7 +9971,7 @@
       <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3">
         <v>18987</v>
       </c>
     </row>
@@ -7989,7 +9985,7 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4">
         <v>18966</v>
       </c>
     </row>
@@ -8003,7 +9999,7 @@
       <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5">
         <v>18566</v>
       </c>
     </row>
@@ -8017,7 +10013,7 @@
       <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6">
         <v>18255</v>
       </c>
     </row>
@@ -8031,7 +10027,7 @@
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7">
         <v>17539</v>
       </c>
     </row>
@@ -8045,7 +10041,7 @@
       <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8">
         <v>16974</v>
       </c>
     </row>
@@ -8059,7 +10055,7 @@
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9">
         <v>16038</v>
       </c>
     </row>
@@ -8073,7 +10069,7 @@
       <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10">
         <v>15742</v>
       </c>
     </row>
@@ -8087,7 +10083,7 @@
       <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11">
         <v>15305</v>
       </c>
     </row>
@@ -8101,7 +10097,7 @@
       <c r="E12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12">
         <v>14258</v>
       </c>
     </row>
@@ -8115,7 +10111,7 @@
       <c r="E13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13">
         <v>12888</v>
       </c>
     </row>
@@ -8123,11 +10119,11 @@
       <c r="E14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14">
         <v>202536</v>
       </c>
     </row>
-    <row r="17" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -8136,17 +10132,8 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-    </row>
-    <row r="18" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -8155,17 +10142,8 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-    </row>
-    <row r="19" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -8174,17 +10152,8 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-    </row>
-    <row r="20" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -8193,17 +10162,8 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
-    </row>
-    <row r="21" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -8212,17 +10172,8 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-    </row>
-    <row r="22" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -8231,17 +10182,8 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
-    </row>
-    <row r="23" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -8250,17 +10192,8 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-    </row>
-    <row r="24" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -8269,17 +10202,8 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-    </row>
-    <row r="25" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -8288,17 +10212,8 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-    </row>
-    <row r="26" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -8307,17 +10222,8 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-    </row>
-    <row r="27" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -8326,17 +10232,8 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
-      <c r="U27" s="5"/>
-    </row>
-    <row r="28" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -8345,17 +10242,8 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
-    </row>
-    <row r="29" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -8364,17 +10252,8 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
-    </row>
-    <row r="30" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -8383,17 +10262,8 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
-      <c r="U30" s="5"/>
-    </row>
-    <row r="31" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -8402,17 +10272,8 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-    </row>
-    <row r="32" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -8421,26 +10282,6 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-    </row>
-    <row r="33" spans="13:21" x14ac:dyDescent="0.25">
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="5"/>
-      <c r="U33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding bar chart to hottest vs coldest day
</commit_message>
<xml_diff>
--- a/excel/sql_query_output.xlsx
+++ b/excel/sql_query_output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime\Desktop\git-repo\chicago_crime_and_weather_2021\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2A005E7-00F5-43A9-A368-4C94B94A4BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D194AD-9580-4EB3-8223-C0B2ABB4CFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="6" activeTab="9" xr2:uid="{CE6839DA-4336-434C-A3C6-5CF43E49803F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{CE6839DA-4336-434C-A3C6-5CF43E49803F}"/>
   </bookViews>
   <sheets>
     <sheet name="consecutive_homicide" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,8 @@
     <pivotCache cacheId="0" r:id="rId14"/>
     <pivotCache cacheId="1" r:id="rId15"/>
     <pivotCache cacheId="2" r:id="rId16"/>
-    <pivotCache cacheId="5" r:id="rId17"/>
+    <pivotCache cacheId="3" r:id="rId17"/>
+    <pivotCache cacheId="9" r:id="rId18"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -109,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="98">
   <si>
     <t>most_consecutive_days</t>
   </si>
@@ -395,18 +396,44 @@
   <si>
     <t>North Park</t>
   </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+  </si>
+  <si>
+    <t>95°</t>
+  </si>
+  <si>
+    <t>4°</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -480,6 +507,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF90170A"/>
+      <color rgb="FFFC5736"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1324,6 +1357,484 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
+    <c:name>[sql_query_output.xlsx]hottest_vs_coldest!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:gradFill>
+            <a:gsLst>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="5000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="45000"/>
+                  <a:lumOff val="55000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:gradFill>
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:srgbClr val="FC5736"/>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:srgbClr val="90170A"/>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.2553191489361701E-2"/>
+          <c:y val="9.0909199366737498E-2"/>
+          <c:w val="0.89598108747044913"/>
+          <c:h val="0.71979804318544882"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hottest_vs_coldest!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="5000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="45000"/>
+                      <a:lumOff val="55000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="1"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-24E4-4D00-99A0-996B90944AD8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:srgbClr val="FC5736"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:srgbClr val="90170A"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="1"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-24E4-4D00-99A0-996B90944AD8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>hottest_vs_coldest!$D$3:$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4°</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95°</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>hottest_vs_coldest!$E$3:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>552</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-24E4-4D00-99A0-996B90944AD8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1406412112"/>
+        <c:axId val="1406409616"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1406412112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1406409616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1406409616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1406412112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
     <c:name>[sql_query_output.xlsx]top_crime_month!PivotTable1</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
@@ -1714,7 +2225,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2297,7 +2808,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3294,6 +3805,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3798,7 +4349,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4002,6 +4553,509 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -4302,7 +5356,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4805,7 +5859,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5548,6 +6602,338 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>42859</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="13" name="Group 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61078A65-8B46-3949-3CA3-C67743EA6CF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2066925" y="1947859"/>
+          <a:ext cx="3781425" cy="1947866"/>
+          <a:chOff x="6610350" y="2624134"/>
+          <a:chExt cx="3781425" cy="1947866"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99D5336C-2F7E-8E47-4888-E056C1D96A18}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6610350" y="2628899"/>
+            <a:ext cx="3781425" cy="1943101"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 3261"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="2" name="Chart 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C631A2AC-8E89-49C3-1647-BCEEAF179351}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="8124825" y="3238501"/>
+          <a:ext cx="2247900" cy="1304924"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="9" name="Graphic 8" descr="Snow outline">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9F3B018-1E62-DA3C-FC5D-5C82A44F6B27}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8391526" y="2655076"/>
+            <a:ext cx="676274" cy="676274"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="Graphic 4" descr="High temperature outline">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F4FB73A-53E3-A180-600F-C4C2E3FA0FC5}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId5"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9486900" y="2683649"/>
+            <a:ext cx="466725" cy="466725"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Rectangle: Top Corners Rounded 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44FD18FF-EB54-FD3D-7711-29A4C48FAE97}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="6472237" y="2786061"/>
+            <a:ext cx="1947865" cy="1624011"/>
+          </a:xfrm>
+          <a:prstGeom prst="round2SameRect">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 6411"/>
+              <a:gd name="adj2" fmla="val 0"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="TextBox 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39EE6C12-5E9C-36AD-0C2C-4FFA4ABEDDD9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6705600" y="2914650"/>
+            <a:ext cx="1543050" cy="1219565"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>There was a 37% </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FFFF00"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>increase</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> in reported crimes on the hottest day of the year vs. the coldest day of the year.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5802,7 +7188,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6218,7 +7604,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6692,6 +8078,32 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jaime" refreshedDate="44940.377409490742" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{4DB5EAF7-3764-4519-823E-3C7E32C3CBB8}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="hottest_vs_coldest"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="temp_high" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="95" count="4">
+        <s v="4°"/>
+        <s v="95°"/>
+        <n v="95" u="1"/>
+        <n v="4" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="n_crimes" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="402" maxValue="552"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
@@ -6864,6 +8276,19 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="2">
+  <r>
+    <x v="0"/>
+    <n v="402"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="552"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7400F035-ADCB-442E-9D3B-CA40FF32DF26}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D2:E3" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
@@ -6940,6 +8365,112 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B967FBB2-071F-4C2C-9B33-121C9D861B34}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="D2:E5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item m="1" x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of n_crimes" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5A4A6DBA-0D8C-4A4F-8EF1-B3A800D707D7}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="E1:F14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
@@ -7035,8 +8566,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{26D5272B-BB1B-4B4D-BF77-AE571D1AD95F}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{26D5272B-BB1B-4B4D-BF77-AE571D1AD95F}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D2:E10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -7147,7 +8678,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{898CC059-EB55-48E2-9B84-1F77F30BA893}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="F2:H15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
@@ -7897,7 +9428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E22186-5F97-42B1-88D0-FEB851F60869}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -7941,7 +9472,7 @@
       <c r="D3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3">
         <v>29569</v>
       </c>
     </row>
@@ -7955,7 +9486,7 @@
       <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>29841</v>
       </c>
     </row>
@@ -7969,7 +9500,7 @@
       <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>29829</v>
       </c>
     </row>
@@ -7983,7 +9514,7 @@
       <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>27825</v>
       </c>
     </row>
@@ -7997,7 +9528,7 @@
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>28143</v>
       </c>
     </row>
@@ -8011,7 +9542,7 @@
       <c r="D8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8">
         <v>28135</v>
       </c>
     </row>
@@ -8019,7 +9550,7 @@
       <c r="D9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9">
         <v>29194</v>
       </c>
     </row>
@@ -8027,7 +9558,7 @@
       <c r="D10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10">
         <v>202536</v>
       </c>
     </row>
@@ -8827,7 +10358,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9054,19 +10585,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAB6722-AE20-4299-94AA-9304ED76D21C}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -9074,26 +10607,182 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>4</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>95</v>
       </c>
       <c r="B2">
         <v>402</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>95</v>
+      <c r="D2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>96</v>
       </c>
       <c r="B3">
         <v>552</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="4">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="4">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="4">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -9103,7 +10792,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9111,6 +10800,10 @@
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="26" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding some flair to bar chart and replacing old png
</commit_message>
<xml_diff>
--- a/excel/sql_query_output.xlsx
+++ b/excel/sql_query_output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime\Desktop\git-repo\chicago_crime_and_weather_2021\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D194AD-9580-4EB3-8223-C0B2ABB4CFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9251730A-7A51-49BF-8FE9-2AAC37624215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{CE6839DA-4336-434C-A3C6-5CF43E49803F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{CE6839DA-4336-434C-A3C6-5CF43E49803F}"/>
   </bookViews>
   <sheets>
     <sheet name="consecutive_homicide" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <pivotCache cacheId="1" r:id="rId15"/>
     <pivotCache cacheId="2" r:id="rId16"/>
     <pivotCache cacheId="3" r:id="rId17"/>
-    <pivotCache cacheId="9" r:id="rId18"/>
+    <pivotCache cacheId="4" r:id="rId18"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -462,14 +462,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6930,6 +6929,116 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{381DE84B-446D-24EB-98AF-AD44E5EEB98F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2209800" y="2133600"/>
+          <a:ext cx="1409700" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FA143DA-6772-40BF-8DD3-8D333CBD2F15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2200275" y="3705225"/>
+          <a:ext cx="1409700" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8365,7 +8474,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B967FBB2-071F-4C2C-9B33-121C9D861B34}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B967FBB2-071F-4C2C-9B33-121C9D861B34}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D2:E5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -9390,8 +9499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C880DC-E1D7-461E-BF95-7779EC04FFB3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10585,10 +10694,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAB6722-AE20-4299-94AA-9304ED76D21C}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10631,7 +10740,7 @@
       <c r="D3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3">
         <v>402</v>
       </c>
     </row>
@@ -10639,7 +10748,7 @@
       <c r="D4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>552</v>
       </c>
     </row>
@@ -10647,7 +10756,7 @@
       <c r="D5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>954</v>
       </c>
     </row>
@@ -10767,15 +10876,6 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>